<commit_message>
apply a no uuid filter
</commit_message>
<xml_diff>
--- a/Documentation/calculator_distance_rssi.xlsx
+++ b/Documentation/calculator_distance_rssi.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="90" windowWidth="27315" windowHeight="9030"/>
+    <workbookView xWindow="600" yWindow="96" windowWidth="27312" windowHeight="9036" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Calculator rssi ecuation:</t>
   </si>
@@ -25,6 +25,18 @@
   </si>
   <si>
     <t>rssi (abs)</t>
+  </si>
+  <si>
+    <t>Scan BLE 2 s</t>
+  </si>
+  <si>
+    <t>time (ms)</t>
+  </si>
+  <si>
+    <t>5 devices find two publisg</t>
+  </si>
+  <si>
+    <t>Time on connected</t>
   </si>
 </sst>
 </file>
@@ -194,11 +206,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="47740800"/>
-        <c:axId val="47739264"/>
+        <c:axId val="205201408"/>
+        <c:axId val="205202944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="47740800"/>
+        <c:axId val="205201408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -208,12 +220,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47739264"/>
+        <c:crossAx val="205202944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="47739264"/>
+        <c:axId val="205202944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -224,7 +236,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47740800"/>
+        <c:crossAx val="205201408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -376,11 +388,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="48329088"/>
-        <c:axId val="48126592"/>
+        <c:axId val="205240192"/>
+        <c:axId val="205241728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48329088"/>
+        <c:axId val="205240192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -390,12 +402,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48126592"/>
+        <c:crossAx val="205241728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48126592"/>
+        <c:axId val="205241728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -406,7 +418,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48329088"/>
+        <c:crossAx val="205240192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -414,6 +426,470 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10015507436570428"/>
+          <c:y val="5.1400554097404488E-2"/>
+          <c:w val="0.78663413179628305"/>
+          <c:h val="0.8326195683872849"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:radarChart>
+        <c:radarStyle val="marker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja2!$B$6:$B$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="56"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja2!$C$6:$C$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="56"/>
+                <c:pt idx="0">
+                  <c:v>5855</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4815</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4862</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4841</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6360</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4831</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4816</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4863</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4820</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5337</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4862</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4848</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5865</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5314</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6856</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6806</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4867</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6880</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6848</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5356</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6368</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4822</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6797</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4862</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4859</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4813</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4883</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4886</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4817</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4866</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4797</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4817</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4858</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4909</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4817</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4815</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4804</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4871</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4874</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4997</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4855</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4856</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4862</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>7513</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4867</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4816</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4855</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4926</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4869</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>6807</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4850</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4866</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4797</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4817</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4858</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4909</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="34691712"/>
+        <c:axId val="36977280"/>
+      </c:radarChart>
+      <c:catAx>
+        <c:axId val="34691712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="36977280"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="36977280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="34691712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.84313887662551767"/>
+          <c:y val="0.93776273655448239"/>
+          <c:w val="0.14030091518900806"/>
+          <c:h val="4.9487995035103371E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -485,6 +961,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>148590</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="1 Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -782,13 +1293,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
@@ -932,13 +1443,481 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B4:G61"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>5855</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>4815</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>4862</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>4841</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>6360</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>4831</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>4816</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>4863</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>4820</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>5337</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>11</v>
+      </c>
+      <c r="C16">
+        <v>4862</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <v>4848</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <v>5865</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>14</v>
+      </c>
+      <c r="C19">
+        <v>5314</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>15</v>
+      </c>
+      <c r="C20">
+        <v>6856</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>16</v>
+      </c>
+      <c r="C21">
+        <v>6806</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>17</v>
+      </c>
+      <c r="C22">
+        <v>4867</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>18</v>
+      </c>
+      <c r="C23">
+        <v>6880</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>19</v>
+      </c>
+      <c r="C24">
+        <v>6848</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>20</v>
+      </c>
+      <c r="C25">
+        <v>5356</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>21</v>
+      </c>
+      <c r="C26">
+        <v>6368</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>22</v>
+      </c>
+      <c r="C27">
+        <v>4822</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>23</v>
+      </c>
+      <c r="C28">
+        <v>6797</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>24</v>
+      </c>
+      <c r="C29">
+        <v>4862</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>25</v>
+      </c>
+      <c r="C30">
+        <v>4859</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>26</v>
+      </c>
+      <c r="C31">
+        <v>4813</v>
+      </c>
+      <c r="G31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>27</v>
+      </c>
+      <c r="C32">
+        <v>4883</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>28</v>
+      </c>
+      <c r="C33">
+        <v>4886</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>29</v>
+      </c>
+      <c r="C34">
+        <v>4817</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>30</v>
+      </c>
+      <c r="C35">
+        <v>4866</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>31</v>
+      </c>
+      <c r="C36">
+        <v>4797</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <v>32</v>
+      </c>
+      <c r="C37">
+        <v>4817</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>33</v>
+      </c>
+      <c r="C38">
+        <v>4858</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <v>34</v>
+      </c>
+      <c r="C39">
+        <v>4909</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>35</v>
+      </c>
+      <c r="C40">
+        <v>4817</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>36</v>
+      </c>
+      <c r="C41">
+        <v>4815</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>37</v>
+      </c>
+      <c r="C42">
+        <v>4804</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <v>38</v>
+      </c>
+      <c r="C43">
+        <v>4871</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>39</v>
+      </c>
+      <c r="C44">
+        <v>4874</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <v>40</v>
+      </c>
+      <c r="C45">
+        <v>4997</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <v>41</v>
+      </c>
+      <c r="C46">
+        <v>4855</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B47">
+        <v>42</v>
+      </c>
+      <c r="C47">
+        <v>4856</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B48">
+        <v>43</v>
+      </c>
+      <c r="C48">
+        <v>4862</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B49">
+        <v>44</v>
+      </c>
+      <c r="C49">
+        <v>7513</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B50">
+        <v>45</v>
+      </c>
+      <c r="C50">
+        <v>4867</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B51">
+        <v>46</v>
+      </c>
+      <c r="C51">
+        <v>4816</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B52">
+        <v>47</v>
+      </c>
+      <c r="C52">
+        <v>4855</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B53">
+        <v>48</v>
+      </c>
+      <c r="C53">
+        <v>4926</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B54">
+        <v>49</v>
+      </c>
+      <c r="C54">
+        <v>4869</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B55">
+        <v>50</v>
+      </c>
+      <c r="C55">
+        <v>6807</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B56">
+        <v>51</v>
+      </c>
+      <c r="C56">
+        <v>4850</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B57">
+        <v>52</v>
+      </c>
+      <c r="C57">
+        <v>4866</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B58">
+        <v>53</v>
+      </c>
+      <c r="C58">
+        <v>4797</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B59">
+        <v>54</v>
+      </c>
+      <c r="C59">
+        <v>4817</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B60">
+        <v>55</v>
+      </c>
+      <c r="C60">
+        <v>4858</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B61">
+        <v>56</v>
+      </c>
+      <c r="C61">
+        <v>4909</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -948,7 +1927,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
3/5 of the memmory
</commit_message>
<xml_diff>
--- a/Documentation/calculator_distance_rssi.xlsx
+++ b/Documentation/calculator_distance_rssi.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Calculator rssi ecuation:</t>
   </si>
@@ -38,12 +38,51 @@
   <si>
     <t>Time on connected</t>
   </si>
+  <si>
+    <t>Consumo Despierto</t>
+  </si>
+  <si>
+    <t>Consumo Dormido</t>
+  </si>
+  <si>
+    <t>Consumo(mA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consumo medio: </t>
+  </si>
+  <si>
+    <t>Envio cada x min</t>
+  </si>
+  <si>
+    <t>Duración en función de batería (días)</t>
+  </si>
+  <si>
+    <t>Tiempo en segundos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pila AA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Batería Li Ion </t>
+  </si>
+  <si>
+    <t>mAh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pila CRC 2032 </t>
+  </si>
+  <si>
+    <t>mA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -51,16 +90,94 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -68,15 +185,203 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="6" borderId="6" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="6" borderId="9" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="20% - Énfasis1" xfId="4" builtinId="30"/>
+    <cellStyle name="40% - Énfasis1" xfId="5" builtinId="31"/>
+    <cellStyle name="40% - Énfasis2" xfId="6" builtinId="35"/>
+    <cellStyle name="Buena" xfId="2" builtinId="26"/>
+    <cellStyle name="Énfasis1" xfId="3" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -206,11 +511,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="205201408"/>
-        <c:axId val="205202944"/>
+        <c:axId val="210059264"/>
+        <c:axId val="210060800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="205201408"/>
+        <c:axId val="210059264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -220,12 +525,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="205202944"/>
+        <c:crossAx val="210060800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="205202944"/>
+        <c:axId val="210060800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -236,14 +541,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="205201408"/>
+        <c:crossAx val="210059264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -388,11 +692,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="205240192"/>
-        <c:axId val="205241728"/>
+        <c:axId val="210098048"/>
+        <c:axId val="210099584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="205240192"/>
+        <c:axId val="210098048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -402,12 +706,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="205241728"/>
+        <c:crossAx val="210099584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="205241728"/>
+        <c:axId val="210099584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -418,14 +722,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="205240192"/>
+        <c:crossAx val="210098048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -839,11 +1142,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="34691712"/>
-        <c:axId val="36977280"/>
+        <c:axId val="210554880"/>
+        <c:axId val="210556416"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="34691712"/>
+        <c:axId val="210554880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -854,7 +1157,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="36977280"/>
+        <c:crossAx val="210556416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -862,7 +1165,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="36977280"/>
+        <c:axId val="210556416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -873,7 +1176,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="34691712"/>
+        <c:crossAx val="210554880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -973,16 +1276,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>148590</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331470</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1443,15 +1746,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:G61"/>
+  <dimension ref="B2:U61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13:O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="N2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>3</v>
       </c>
@@ -1459,28 +1778,73 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="M5" s="1"/>
+      <c r="N5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6">
         <v>5855</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="M6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N6" s="1">
+        <v>120</v>
+      </c>
+      <c r="O6" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="P6" s="3">
+        <f>O6/(60*$O$2)</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="3"/>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7">
         <v>4815</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="M7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N7" s="1">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="O7" s="1">
+        <f>60*O2-(O6)</f>
+        <v>298.8</v>
+      </c>
+      <c r="P7" s="3">
+        <f>O7/(60*$O$2)</f>
+        <v>0.996</v>
+      </c>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="3"/>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>3</v>
       </c>
@@ -1488,7 +1852,7 @@
         <v>4862</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>4</v>
       </c>
@@ -1496,15 +1860,27 @@
         <v>4841</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:21" ht="18" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>5</v>
       </c>
       <c r="C10">
         <v>6360</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="M10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N10" s="8">
+        <f>P6*N6 + N7*P7</f>
+        <v>0.49493999999999999</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+    </row>
+    <row r="11" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>6</v>
       </c>
@@ -1512,39 +1888,76 @@
         <v>4831</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>7</v>
       </c>
       <c r="C12">
         <v>4816</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="M12" s="9"/>
+      <c r="N12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="O12" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>8</v>
       </c>
       <c r="C13">
         <v>4863</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="M13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="N13" s="13">
+        <v>240</v>
+      </c>
+      <c r="O13" s="14">
+        <f>(N13/$N$10)/24</f>
+        <v>20.204469228593364</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>9</v>
       </c>
       <c r="C14">
         <v>4820</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="M14" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="N14" s="13">
+        <v>2500</v>
+      </c>
+      <c r="O14" s="14">
+        <f t="shared" ref="O14:O15" si="0">(N14/$N$10)/24</f>
+        <v>210.46322113118092</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15">
         <v>10</v>
       </c>
       <c r="C15">
         <v>5337</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="M15" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="N15" s="16">
+        <v>1600</v>
+      </c>
+      <c r="O15" s="17">
+        <f t="shared" si="0"/>
+        <v>134.69646152395578</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>11</v>
       </c>
@@ -1917,7 +2330,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
BLE scanners and senders via ESPnow
</commit_message>
<xml_diff>
--- a/Documentation/calculator_distance_rssi.xlsx
+++ b/Documentation/calculator_distance_rssi.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="96" windowWidth="27312" windowHeight="9036" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="90" windowWidth="27315" windowHeight="9030" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>Calculator rssi ecuation:</t>
   </si>
@@ -27,16 +27,7 @@
     <t>rssi (abs)</t>
   </si>
   <si>
-    <t>Scan BLE 2 s</t>
-  </si>
-  <si>
     <t>time (ms)</t>
-  </si>
-  <si>
-    <t>5 devices find two publisg</t>
-  </si>
-  <si>
-    <t>Time on connected</t>
   </si>
   <si>
     <t>Consumo Despierto</t>
@@ -74,15 +65,33 @@
   <si>
     <t>mA</t>
   </si>
+  <si>
+    <t>Scan BLE 2 s and publish via mqtt</t>
+  </si>
+  <si>
+    <t>Scan BLE 2s and send ESP-NOW message</t>
+  </si>
+  <si>
+    <t>Promedio tiempo MQTT</t>
+  </si>
+  <si>
+    <t>MQTT</t>
+  </si>
+  <si>
+    <t>ESP NOW</t>
+  </si>
+  <si>
+    <t>(ms)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,8 +143,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,8 +193,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -320,8 +342,122 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -329,13 +465,13 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -343,9 +479,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -373,14 +506,63 @@
     <xf numFmtId="1" fontId="1" fillId="6" borderId="9" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="8" borderId="10" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="20% - Énfasis1" xfId="4" builtinId="30"/>
     <cellStyle name="40% - Énfasis1" xfId="5" builtinId="31"/>
     <cellStyle name="40% - Énfasis2" xfId="6" builtinId="35"/>
     <cellStyle name="Buena" xfId="2" builtinId="26"/>
     <cellStyle name="Énfasis1" xfId="3" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Notas" xfId="7" builtinId="10"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -511,11 +693,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="210059264"/>
-        <c:axId val="210060800"/>
+        <c:axId val="207171968"/>
+        <c:axId val="207173504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="210059264"/>
+        <c:axId val="207171968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -525,12 +707,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210060800"/>
+        <c:crossAx val="207173504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="210060800"/>
+        <c:axId val="207173504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -541,7 +723,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210059264"/>
+        <c:crossAx val="207171968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -692,11 +874,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="210098048"/>
-        <c:axId val="210099584"/>
+        <c:axId val="207194368"/>
+        <c:axId val="207212544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="210098048"/>
+        <c:axId val="207194368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -706,12 +888,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210099584"/>
+        <c:crossAx val="207212544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="210099584"/>
+        <c:axId val="207212544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -722,7 +904,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210098048"/>
+        <c:crossAx val="207194368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -757,25 +939,50 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>Promedio</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-ES" baseline="0"/>
+              <a:t> de tiempo: barrido BLE 2s + envio datos</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.10015507436570428"/>
-          <c:y val="5.1400554097404488E-2"/>
-          <c:w val="0.78663413179628305"/>
-          <c:h val="0.8326195683872849"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:radarChart>
         <c:radarStyle val="marker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja2!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Scan BLE 2 s and publish via mqtt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -1129,6 +1336,201 @@
                 </c:pt>
                 <c:pt idx="55">
                   <c:v>4909</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja2!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Scan BLE 2s and send ESP-NOW message</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja2!$E$6:$E$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="56"/>
+                <c:pt idx="0">
+                  <c:v>2634</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2677</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2635</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2633</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2637</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2647</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2632</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2639</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2632</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2632</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2715</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2635</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2629</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2627</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2641</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2632</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2635</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2632</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2635</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2632</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2632</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2715</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2633</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2637</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2635</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2629</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2633</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2637</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2647</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2623</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2715</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2630</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2627</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2642</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2634</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2632</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2620</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2705</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2649</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2632</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2627</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2641</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2632</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2632</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2632</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2637</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2718</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2639</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2632</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2629</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2637</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2647</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2623</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2715</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2633</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2637</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1142,11 +1544,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="210554880"/>
-        <c:axId val="210556416"/>
+        <c:axId val="207745792"/>
+        <c:axId val="207747328"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="210554880"/>
+        <c:axId val="207745792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1154,10 +1556,15 @@
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210556416"/>
+        <c:spPr>
+          <a:ln w="9525">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="207747328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1165,7 +1572,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="210556416"/>
+        <c:axId val="207747328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1173,27 +1580,40 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210554880"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="207745792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.84313887662551767"/>
-          <c:y val="0.93776273655448239"/>
-          <c:w val="0.14030091518900806"/>
-          <c:h val="4.9487995035103371E-2"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:ln w="41275"/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400"/>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -1276,16 +1696,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>331470</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>502919</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>20955</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1733550</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1600,9 +2020,9 @@
       <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
@@ -1748,587 +2168,1121 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13:O15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T48" sqref="T48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="18.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="0.5703125" customWidth="1"/>
     <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="O2" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
+    <row r="2" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="4">
+        <v>10</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="T2" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="M4" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" s="28"/>
+      <c r="O4" s="29"/>
+      <c r="R4" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="S4" s="28"/>
+      <c r="T4" s="29"/>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-    </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="E5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="17"/>
+      <c r="N5" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="O5" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="R5" s="17"/>
+      <c r="S5" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="T5" s="19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>5855</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N6" s="1">
+      <c r="D6" s="1">
+        <v>2666</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" ref="E6:E37" si="0">D6-32</f>
+        <v>2634</v>
+      </c>
+      <c r="G6" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="31"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="16">
+        <f>AVERAGE(C6:C61)</f>
+        <v>5227.8035714285716</v>
+      </c>
+      <c r="M6" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="N6" s="18">
         <v>120</v>
       </c>
-      <c r="O6" s="1">
-        <v>1.2</v>
-      </c>
-      <c r="P6" s="3">
+      <c r="O6" s="19">
+        <f>J6*0.001</f>
+        <v>5.2278035714285718</v>
+      </c>
+      <c r="P6" s="2">
         <f>O6/(60*$O$2)</f>
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="3"/>
-    </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.3">
+        <v>8.713005952380953E-3</v>
+      </c>
+      <c r="R6" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="S6" s="18">
+        <v>120</v>
+      </c>
+      <c r="T6" s="19">
+        <f>J7*0.001</f>
+        <v>2.6433750000000003</v>
+      </c>
+      <c r="U6" s="2">
+        <f>T6/(60*$O$2)</f>
+        <v>4.4056250000000007E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>2</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>4815</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N7" s="1">
+      <c r="D7" s="1">
+        <v>2709</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>2677</v>
+      </c>
+      <c r="G7" s="32"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="16">
+        <f>AVERAGE(E6:E61)</f>
+        <v>2643.375</v>
+      </c>
+      <c r="M7" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="N7" s="18">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="O7" s="1">
+      <c r="O7" s="19">
         <f>60*O2-(O6)</f>
-        <v>298.8</v>
-      </c>
-      <c r="P7" s="3">
+        <v>594.77219642857142</v>
+      </c>
+      <c r="P7" s="2">
         <f>O7/(60*$O$2)</f>
-        <v>0.996</v>
-      </c>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="3"/>
-    </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
+        <v>0.991286994047619</v>
+      </c>
+      <c r="R7" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="S7" s="18">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="T7" s="19">
+        <f>60*T2-(T6)</f>
+        <v>597.35662500000001</v>
+      </c>
+      <c r="U7" s="2">
+        <f>T7/(60*$O$2)</f>
+        <v>0.99559437500000003</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>3</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>4862</v>
       </c>
-    </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="D8" s="1">
+        <v>2667</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>2635</v>
+      </c>
+      <c r="M8" s="20"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="22"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="22"/>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>4</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>4841</v>
       </c>
-    </row>
-    <row r="10" spans="2:21" ht="18" x14ac:dyDescent="0.35">
+      <c r="D9" s="1">
+        <v>2665</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>2633</v>
+      </c>
+      <c r="M9" s="20"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="22"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="21"/>
+      <c r="T9" s="22"/>
+    </row>
+    <row r="10" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>5</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>6360</v>
       </c>
-      <c r="M10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="N10" s="8">
+      <c r="D10" s="1">
+        <v>2669</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="0"/>
+        <v>2637</v>
+      </c>
+      <c r="M10" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="N10" s="24">
         <f>P6*N6 + N7*P7</f>
-        <v>0.49493999999999999</v>
-      </c>
-      <c r="O10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-    </row>
-    <row r="11" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>1.0604300191964287</v>
+      </c>
+      <c r="O10" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="R10" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="S10" s="24">
+        <f>U6*S6 + S7*U7</f>
+        <v>0.54360891562500013</v>
+      </c>
+      <c r="T10" s="25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>6</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>4831</v>
       </c>
-    </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="D11" s="1">
+        <v>2679</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="0"/>
+        <v>2647</v>
+      </c>
+      <c r="M11" s="20"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="22"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="22"/>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>7</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>4816</v>
       </c>
-      <c r="M12" s="9"/>
-      <c r="N12" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="O12" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="D12" s="1">
+        <v>2664</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="0"/>
+        <v>2632</v>
+      </c>
+      <c r="M12" s="5"/>
+      <c r="N12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="R12" s="5"/>
+      <c r="S12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="T12" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>8</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>4863</v>
       </c>
-      <c r="M13" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="N13" s="13">
+      <c r="D13" s="1">
+        <v>2671</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="0"/>
+        <v>2639</v>
+      </c>
+      <c r="M13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N13" s="9">
         <v>240</v>
       </c>
-      <c r="O13" s="14">
+      <c r="O13" s="10">
         <f>(N13/$N$10)/24</f>
-        <v>20.204469228593364</v>
-      </c>
-    </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.3">
+        <v>9.4301366605764212</v>
+      </c>
+      <c r="R13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="S13" s="9">
+        <v>240</v>
+      </c>
+      <c r="T13" s="10">
+        <f>(S13/$S$10)/24</f>
+        <v>18.395577615762175</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>9</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>4820</v>
       </c>
-      <c r="M14" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="N14" s="13">
+      <c r="D14" s="1">
+        <v>2664</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="0"/>
+        <v>2632</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="N14" s="9">
         <v>2500</v>
       </c>
-      <c r="O14" s="14">
-        <f t="shared" ref="O14:O15" si="0">(N14/$N$10)/24</f>
-        <v>210.46322113118092</v>
-      </c>
-    </row>
-    <row r="15" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="O14" s="10">
+        <f t="shared" ref="O14:O15" si="1">(N14/$N$10)/24</f>
+        <v>98.230590214337724</v>
+      </c>
+      <c r="R14" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="S14" s="9">
+        <v>2500</v>
+      </c>
+      <c r="T14" s="10">
+        <f t="shared" ref="T14:T15" si="2">(S14/$S$10)/24</f>
+        <v>191.62060016418931</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>10</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>5337</v>
       </c>
-      <c r="M15" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="N15" s="16">
+      <c r="D15" s="1">
+        <v>2664</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="0"/>
+        <v>2632</v>
+      </c>
+      <c r="M15" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="N15" s="12">
         <v>1600</v>
       </c>
-      <c r="O15" s="17">
-        <f t="shared" si="0"/>
-        <v>134.69646152395578</v>
-      </c>
-    </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="O15" s="13">
+        <f t="shared" si="1"/>
+        <v>62.867577737176141</v>
+      </c>
+      <c r="R15" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="S15" s="12">
+        <v>1600</v>
+      </c>
+      <c r="T15" s="13">
+        <f t="shared" si="2"/>
+        <v>122.63718410508115</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>11</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>4862</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D16" s="1">
+        <v>2747</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="0"/>
+        <v>2715</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>12</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>4848</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D17" s="1">
+        <v>2667</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="0"/>
+        <v>2635</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>13</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>5865</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D18" s="1">
+        <v>2661</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="0"/>
+        <v>2629</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>14</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>5314</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D19" s="1">
+        <v>2659</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="0"/>
+        <v>2627</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>15</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="1">
         <v>6856</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D20" s="1">
+        <v>2673</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="0"/>
+        <v>2641</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>16</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <v>6806</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D21" s="1">
+        <v>2664</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="0"/>
+        <v>2632</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>17</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <v>4867</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D22" s="1">
+        <v>2667</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="0"/>
+        <v>2635</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>18</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>6880</v>
       </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D23" s="1">
+        <v>2664</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="0"/>
+        <v>2632</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>19</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="1">
         <v>6848</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D24" s="1">
+        <v>2667</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="0"/>
+        <v>2635</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>20</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="1">
         <v>5356</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D25" s="1">
+        <v>2664</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="0"/>
+        <v>2632</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>21</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
         <v>6368</v>
       </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D26" s="1">
+        <v>2664</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="0"/>
+        <v>2632</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>22</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="1">
         <v>4822</v>
       </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D27" s="1">
+        <v>2747</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="0"/>
+        <v>2715</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>23</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="1">
         <v>6797</v>
       </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D28" s="1">
+        <v>2665</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" si="0"/>
+        <v>2633</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>24</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="1">
         <v>4862</v>
       </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D29" s="1">
+        <v>2669</v>
+      </c>
+      <c r="E29" s="1">
+        <f t="shared" si="0"/>
+        <v>2637</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>25</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="1">
         <v>4859</v>
       </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D30" s="1">
+        <v>2667</v>
+      </c>
+      <c r="E30" s="1">
+        <f t="shared" si="0"/>
+        <v>2635</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>26</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="1">
         <v>4813</v>
       </c>
-      <c r="G31" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D31" s="1">
+        <v>2661</v>
+      </c>
+      <c r="E31" s="1">
+        <f t="shared" si="0"/>
+        <v>2629</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>27</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="1">
         <v>4883</v>
       </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D32" s="1">
+        <v>2665</v>
+      </c>
+      <c r="E32" s="1">
+        <f t="shared" si="0"/>
+        <v>2633</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>28</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="1">
         <v>4886</v>
       </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D33" s="1">
+        <v>2669</v>
+      </c>
+      <c r="E33" s="1">
+        <f t="shared" si="0"/>
+        <v>2637</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>29</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="1">
         <v>4817</v>
       </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D34" s="1">
+        <v>2679</v>
+      </c>
+      <c r="E34" s="1">
+        <f t="shared" si="0"/>
+        <v>2647</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>30</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="1">
         <v>4866</v>
       </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D35" s="1">
+        <v>2655</v>
+      </c>
+      <c r="E35" s="1">
+        <f t="shared" si="0"/>
+        <v>2623</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>31</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="1">
         <v>4797</v>
       </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D36" s="1">
+        <v>2747</v>
+      </c>
+      <c r="E36" s="1">
+        <f t="shared" si="0"/>
+        <v>2715</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>32</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="1">
         <v>4817</v>
       </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D37" s="1">
+        <v>2662</v>
+      </c>
+      <c r="E37" s="1">
+        <f t="shared" si="0"/>
+        <v>2630</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>33</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="1">
         <v>4858</v>
       </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D38" s="1">
+        <v>2659</v>
+      </c>
+      <c r="E38" s="1">
+        <f t="shared" ref="E38:E69" si="3">D38-32</f>
+        <v>2627</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>34</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="1">
         <v>4909</v>
       </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D39" s="1">
+        <v>2674</v>
+      </c>
+      <c r="E39" s="1">
+        <f t="shared" si="3"/>
+        <v>2642</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>35</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="1">
         <v>4817</v>
       </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D40" s="1">
+        <v>2666</v>
+      </c>
+      <c r="E40" s="1">
+        <f t="shared" si="3"/>
+        <v>2634</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>36</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="1">
         <v>4815</v>
       </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D41" s="1">
+        <v>2664</v>
+      </c>
+      <c r="E41" s="1">
+        <f t="shared" si="3"/>
+        <v>2632</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>37</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="1">
         <v>4804</v>
       </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D42" s="1">
+        <v>2652</v>
+      </c>
+      <c r="E42" s="1">
+        <f t="shared" si="3"/>
+        <v>2620</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>38</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="1">
         <v>4871</v>
       </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D43" s="1">
+        <v>2737</v>
+      </c>
+      <c r="E43" s="1">
+        <f t="shared" si="3"/>
+        <v>2705</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>39</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="1">
         <v>4874</v>
       </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D44" s="1">
+        <v>2681</v>
+      </c>
+      <c r="E44" s="1">
+        <f t="shared" si="3"/>
+        <v>2649</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>40</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="1">
         <v>4997</v>
       </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D45" s="1">
+        <v>2664</v>
+      </c>
+      <c r="E45" s="1">
+        <f t="shared" si="3"/>
+        <v>2632</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>41</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="1">
         <v>4855</v>
       </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D46" s="1">
+        <v>2659</v>
+      </c>
+      <c r="E46" s="1">
+        <f t="shared" si="3"/>
+        <v>2627</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>42</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="1">
         <v>4856</v>
       </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D47" s="1">
+        <v>2673</v>
+      </c>
+      <c r="E47" s="1">
+        <f t="shared" si="3"/>
+        <v>2641</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>43</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="1">
         <v>4862</v>
       </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D48" s="1">
+        <v>2664</v>
+      </c>
+      <c r="E48" s="1">
+        <f t="shared" si="3"/>
+        <v>2632</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>44</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="1">
         <v>7513</v>
       </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D49" s="1">
+        <v>2664</v>
+      </c>
+      <c r="E49" s="1">
+        <f t="shared" si="3"/>
+        <v>2632</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>45</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="1">
         <v>4867</v>
       </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D50" s="1">
+        <v>2664</v>
+      </c>
+      <c r="E50" s="1">
+        <f t="shared" si="3"/>
+        <v>2632</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>46</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="1">
         <v>4816</v>
       </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D51" s="1">
+        <v>2669</v>
+      </c>
+      <c r="E51" s="1">
+        <f t="shared" si="3"/>
+        <v>2637</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>47</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="1">
         <v>4855</v>
       </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D52" s="1">
+        <v>2750</v>
+      </c>
+      <c r="E52" s="1">
+        <f t="shared" si="3"/>
+        <v>2718</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>48</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="1">
         <v>4926</v>
       </c>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D53" s="1">
+        <v>2671</v>
+      </c>
+      <c r="E53" s="1">
+        <f t="shared" si="3"/>
+        <v>2639</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54">
         <v>49</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="1">
         <v>4869</v>
       </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D54" s="1">
+        <v>2664</v>
+      </c>
+      <c r="E54" s="1">
+        <f t="shared" si="3"/>
+        <v>2632</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55">
         <v>50</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="1">
         <v>6807</v>
       </c>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D55" s="1">
+        <v>2661</v>
+      </c>
+      <c r="E55" s="1">
+        <f t="shared" si="3"/>
+        <v>2629</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56">
         <v>51</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="1">
         <v>4850</v>
       </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D56" s="1">
+        <v>2669</v>
+      </c>
+      <c r="E56" s="1">
+        <f t="shared" si="3"/>
+        <v>2637</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57">
         <v>52</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="1">
         <v>4866</v>
       </c>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D57" s="1">
+        <v>2679</v>
+      </c>
+      <c r="E57" s="1">
+        <f t="shared" si="3"/>
+        <v>2647</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>53</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="1">
         <v>4797</v>
       </c>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D58" s="1">
+        <v>2655</v>
+      </c>
+      <c r="E58" s="1">
+        <f t="shared" si="3"/>
+        <v>2623</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59">
         <v>54</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="1">
         <v>4817</v>
       </c>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D59" s="1">
+        <v>2747</v>
+      </c>
+      <c r="E59" s="1">
+        <f t="shared" si="3"/>
+        <v>2715</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>55</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="1">
         <v>4858</v>
       </c>
-    </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D60" s="1">
+        <v>2665</v>
+      </c>
+      <c r="E60" s="1">
+        <f t="shared" si="3"/>
+        <v>2633</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>56</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="1">
         <v>4909</v>
       </c>
+      <c r="D61" s="1">
+        <v>2669</v>
+      </c>
+      <c r="E61" s="1">
+        <f t="shared" si="3"/>
+        <v>2637</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="G6:H7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -2341,7 +3295,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>